<commit_message>
Update on 20 Jan
</commit_message>
<xml_diff>
--- a/Part2-Regression/Practice/HousePrice_Analysis.xlsx
+++ b/Part2-Regression/Practice/HousePrice_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z003z7n/Documents/AI2019/Part2-Regression/Practice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDF39AF-7649-BC4D-A14F-A377ABA8213D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17870044-CC10-0A48-B9E2-858D05031776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40560" yWindow="2160" windowWidth="27640" windowHeight="16940" xr2:uid="{E3ABDB74-871A-FB42-86A8-3241D447925E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13960" xr2:uid="{E3ABDB74-871A-FB42-86A8-3241D447925E}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns_Analysis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="131">
   <si>
     <t>Column Name</t>
   </si>
@@ -139,6 +139,285 @@
   </si>
   <si>
     <t>Physical locations within Ames city limits</t>
+  </si>
+  <si>
+    <t>Condition1</t>
+  </si>
+  <si>
+    <t>Proximity to various conditions</t>
+  </si>
+  <si>
+    <t>Condition2</t>
+  </si>
+  <si>
+    <t>Proximity to various conditions (if more than one is present)</t>
+  </si>
+  <si>
+    <t>BldgType</t>
+  </si>
+  <si>
+    <t>Type of dwelling</t>
+  </si>
+  <si>
+    <t>HouseStyle</t>
+  </si>
+  <si>
+    <t>Style of dwelling</t>
+  </si>
+  <si>
+    <t>OverallQual</t>
+  </si>
+  <si>
+    <t>Rates the overall material and finish of the house</t>
+  </si>
+  <si>
+    <t>OverallCond</t>
+  </si>
+  <si>
+    <t>Rates the overall condition of the house</t>
+  </si>
+  <si>
+    <t>Of importance</t>
+  </si>
+  <si>
+    <t>YearBuilt</t>
+  </si>
+  <si>
+    <t>Original construction date</t>
+  </si>
+  <si>
+    <t>YearRemodAdd</t>
+  </si>
+  <si>
+    <t>Identified by Numbers (Years)</t>
+  </si>
+  <si>
+    <t>Remodel date (same as construction date if no remodeling or additions)</t>
+  </si>
+  <si>
+    <t>RoofStyle</t>
+  </si>
+  <si>
+    <t>Type of roof</t>
+  </si>
+  <si>
+    <t>RoofMatl</t>
+  </si>
+  <si>
+    <t>Roof material</t>
+  </si>
+  <si>
+    <t>Exterior1st</t>
+  </si>
+  <si>
+    <t>Exterior covering on house</t>
+  </si>
+  <si>
+    <t>Exterior2nd</t>
+  </si>
+  <si>
+    <t>Exterior covering on house (if more than one material)</t>
+  </si>
+  <si>
+    <t>MasVnrType</t>
+  </si>
+  <si>
+    <t>Masonry veneer area in square feet</t>
+  </si>
+  <si>
+    <t>ExterQual</t>
+  </si>
+  <si>
+    <t>Evaluates the quality of the material on the exterior</t>
+  </si>
+  <si>
+    <t>Of importance as it relates to material on the exterior.</t>
+  </si>
+  <si>
+    <t>ExterCond</t>
+  </si>
+  <si>
+    <t>Evaluates the present condition of the material on the exterior</t>
+  </si>
+  <si>
+    <t>Foundation</t>
+  </si>
+  <si>
+    <t>Type of foundation</t>
+  </si>
+  <si>
+    <t>BsmtQual</t>
+  </si>
+  <si>
+    <t>Evaluates the height of the basement</t>
+  </si>
+  <si>
+    <t>BsmtCond</t>
+  </si>
+  <si>
+    <t>Evaluates the general condition of the basement</t>
+  </si>
+  <si>
+    <t>BsmtExposure</t>
+  </si>
+  <si>
+    <t>Refers to walkout or garden level walls</t>
+  </si>
+  <si>
+    <t>BsmtFinType1</t>
+  </si>
+  <si>
+    <t>Rating of basement finished area</t>
+  </si>
+  <si>
+    <t>BsmtFinSF1</t>
+  </si>
+  <si>
+    <t>Type 1 finished square feet</t>
+  </si>
+  <si>
+    <t>BsmtFinType2</t>
+  </si>
+  <si>
+    <t>Rating of basement finished area (if multiple types)</t>
+  </si>
+  <si>
+    <t>BsmtFinSF2</t>
+  </si>
+  <si>
+    <t>Type 2 finished square feet</t>
+  </si>
+  <si>
+    <t>BsmtUnfSF</t>
+  </si>
+  <si>
+    <t>Unfinished square feet of basement area</t>
+  </si>
+  <si>
+    <t>TotalBsmtSF</t>
+  </si>
+  <si>
+    <t>Total square feet of basement area</t>
+  </si>
+  <si>
+    <t>Heating</t>
+  </si>
+  <si>
+    <t>Type of heating</t>
+  </si>
+  <si>
+    <t>HeatingQC</t>
+  </si>
+  <si>
+    <t>Heating quality and condition</t>
+  </si>
+  <si>
+    <t>CentralAir</t>
+  </si>
+  <si>
+    <t>Central air conditioning</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Electrical system</t>
+  </si>
+  <si>
+    <t>1stFlrSF</t>
+  </si>
+  <si>
+    <t>First Floor square feet</t>
+  </si>
+  <si>
+    <t>2ndFlrSF</t>
+  </si>
+  <si>
+    <t>Second floor square feet</t>
+  </si>
+  <si>
+    <t>LowQualFinSF</t>
+  </si>
+  <si>
+    <t>Low quality finished square feet (all floors)</t>
+  </si>
+  <si>
+    <t>GrLivArea</t>
+  </si>
+  <si>
+    <t>Above grade (ground) living area square feet</t>
+  </si>
+  <si>
+    <t>BsmtFullBath</t>
+  </si>
+  <si>
+    <t>Basement full bathrooms</t>
+  </si>
+  <si>
+    <t>BsmtHalfBath</t>
+  </si>
+  <si>
+    <t>Basement half bathrooms</t>
+  </si>
+  <si>
+    <t>FullBath</t>
+  </si>
+  <si>
+    <t>Full bathrooms above grade</t>
+  </si>
+  <si>
+    <t>HalfBath</t>
+  </si>
+  <si>
+    <t>Half baths above grade</t>
+  </si>
+  <si>
+    <t>KitchenQual</t>
+  </si>
+  <si>
+    <t>Kitchen quality</t>
+  </si>
+  <si>
+    <t>TotRmsAbvGrd</t>
+  </si>
+  <si>
+    <t>Total rooms above grade (does not include bathrooms)</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Home functionality (Assume typical unless deductions are warranted)</t>
+  </si>
+  <si>
+    <t>Fireplaces</t>
+  </si>
+  <si>
+    <t>Number of fireplaces</t>
+  </si>
+  <si>
+    <t>FireplaceQu</t>
+  </si>
+  <si>
+    <t>Fireplace quality</t>
+  </si>
+  <si>
+    <t>GarageType</t>
+  </si>
+  <si>
+    <t>Garage location</t>
+  </si>
+  <si>
+    <t>GarageYrBlt</t>
+  </si>
+  <si>
+    <t>Year garage was built</t>
+  </si>
+  <si>
+    <t>GarageFinish</t>
+  </si>
+  <si>
+    <t>Interior finish of the garage</t>
   </si>
 </sst>
 </file>
@@ -512,18 +791,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7307907-8A62-CF45-87CB-25429CB4E75A}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.5" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -725,6 +1004,654 @@
         <v>37</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>